<commit_message>
Réglage bug Rubrique Criteres
</commit_message>
<xml_diff>
--- a/ressource/TestFonctionnel.xlsx
+++ b/ressource/TestFonctionnel.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxime\Documents\GitHub\scrumweek\ressource\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="47">
   <si>
     <t>TEST FONCTIONNEL</t>
   </si>
@@ -163,6 +158,9 @@
   </si>
   <si>
     <t>Pas de confirmation de modification + fermeture de la pop up + duplication du devoir</t>
+  </si>
+  <si>
+    <t>Modifié a 15h (03/07/15)</t>
   </si>
 </sst>
 </file>
@@ -608,7 +606,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -618,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,6 +626,7 @@
     <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="1"/>
     <col min="4" max="4" width="99.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1025,15 +1024,17 @@
         <v>40</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">

</xml_diff>